<commit_message>
benefit_vs_choice analysis & corrections in causal forests
Former-commit-id: a94e41dada3d0ce771362fc224735b66a8842aa5
</commit_message>
<xml_diff>
--- a/Tables/iv_reg_demand_pf.xlsx
+++ b/Tables/iv_reg_demand_pf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B0381B-B7FF-4959-AAB6-B07488640981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEB9451-0DCA-46FC-8F62-B555F862C757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20070" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{218C7A43-1740-403D-A1A7-5BE9A17F8D05}"/>
+    <workbookView xWindow="-17280" yWindow="-6630" windowWidth="14400" windowHeight="8265" xr2:uid="{D78575F0-E3CD-492C-A10C-D3F2CF2BD93E}"/>
   </bookViews>
   <sheets>
     <sheet name="iv_reg_demand_pf" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Observations</t>
   </si>
@@ -45,6 +45,48 @@
     <t>$&gt;$100000</t>
   </si>
   <si>
+    <t>$\sim$100000</t>
+  </si>
+  <si>
+    <t>FP available</t>
+  </si>
+  <si>
+    <t>Had FP in the past</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>OLS</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>IV - 0</t>
+  </si>
+  <si>
+    <t>IV - 1</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>(4)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>Calendar week FE</t>
+  </si>
+  <si>
     <t>\checkmark</t>
   </si>
   <si>
@@ -52,64 +94,16 @@
   </si>
   <si>
     <t>Client FE</t>
-  </si>
-  <si>
-    <t>Calendar week FE</t>
-  </si>
-  <si>
-    <t>Residual</t>
-  </si>
-  <si>
-    <t>FP available</t>
-  </si>
-  <si>
-    <t>Had FP in the past</t>
-  </si>
-  <si>
-    <t>FS</t>
-  </si>
-  <si>
-    <t>OLS</t>
-  </si>
-  <si>
-    <t>IV - 0</t>
-  </si>
-  <si>
-    <t>IV - 1</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>(3)</t>
-  </si>
-  <si>
-    <t>(4)</t>
-  </si>
-  <si>
-    <t>(5)</t>
-  </si>
-  <si>
-    <t>(6)</t>
-  </si>
-  <si>
-    <t>$\sim$100000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,7 +131,20 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -155,33 +162,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -189,14 +180,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -256,9 +253,6 @@
           </cell>
         </row>
         <row r="6">
-          <cell r="A6" t="str">
-            <v/>
-          </cell>
           <cell r="B6" t="str">
             <v>(0.00065)</v>
           </cell>
@@ -278,136 +272,133 @@
             <v/>
           </cell>
         </row>
-        <row r="644">
-          <cell r="B644" t="str">
-            <v/>
-          </cell>
-          <cell r="C644" t="str">
+        <row r="8">
+          <cell r="B8" t="str">
+            <v/>
+          </cell>
+          <cell r="C8" t="str">
             <v>0.49</v>
           </cell>
-          <cell r="D644" t="str">
-            <v/>
-          </cell>
-          <cell r="E644" t="str">
+          <cell r="D8" t="str">
+            <v/>
+          </cell>
+          <cell r="E8" t="str">
             <v>0.30</v>
           </cell>
-          <cell r="G644" t="str">
+          <cell r="G8" t="str">
             <v>0.42</v>
           </cell>
-          <cell r="I644" t="str">
+          <cell r="I8" t="str">
             <v>0.25</v>
           </cell>
         </row>
-        <row r="645">
-          <cell r="A645" t="str">
-            <v/>
-          </cell>
-          <cell r="B645" t="str">
-            <v/>
-          </cell>
-          <cell r="C645" t="str">
+        <row r="9">
+          <cell r="B9" t="str">
+            <v/>
+          </cell>
+          <cell r="C9" t="str">
             <v>(0.071)</v>
           </cell>
-          <cell r="D645" t="str">
-            <v/>
-          </cell>
-          <cell r="E645" t="str">
+          <cell r="D9" t="str">
+            <v/>
+          </cell>
+          <cell r="E9" t="str">
             <v>(0.18)</v>
           </cell>
-          <cell r="G645" t="str">
+          <cell r="G9" t="str">
             <v>(0.076)</v>
           </cell>
-          <cell r="I645" t="str">
+          <cell r="I9" t="str">
             <v>(0.21)</v>
           </cell>
         </row>
-        <row r="647">
-          <cell r="B647" t="str">
-            <v/>
-          </cell>
-          <cell r="C647" t="str">
+        <row r="11">
+          <cell r="B11" t="str">
+            <v/>
+          </cell>
+          <cell r="C11" t="str">
             <v>-0.015</v>
           </cell>
-          <cell r="D647" t="str">
-            <v/>
-          </cell>
-          <cell r="E647" t="str">
+          <cell r="D11" t="str">
+            <v/>
+          </cell>
+          <cell r="E11" t="str">
             <v>-0.51</v>
           </cell>
-          <cell r="G647" t="str">
+          <cell r="G11" t="str">
             <v>0.016</v>
           </cell>
-          <cell r="I647" t="str">
+          <cell r="I11" t="str">
             <v>-0.48</v>
           </cell>
         </row>
-        <row r="648">
-          <cell r="A648" t="str">
-            <v/>
-          </cell>
-          <cell r="B648" t="str">
-            <v/>
-          </cell>
-          <cell r="C648" t="str">
+        <row r="12">
+          <cell r="A12" t="str">
+            <v/>
+          </cell>
+          <cell r="B12" t="str">
+            <v/>
+          </cell>
+          <cell r="C12" t="str">
             <v>(0.070)</v>
           </cell>
-          <cell r="D648" t="str">
-            <v/>
-          </cell>
-          <cell r="E648" t="str">
+          <cell r="D12" t="str">
+            <v/>
+          </cell>
+          <cell r="E12" t="str">
             <v>(0.18)</v>
           </cell>
-          <cell r="G648" t="str">
+          <cell r="G12" t="str">
             <v>(0.075)</v>
           </cell>
-          <cell r="I648" t="str">
+          <cell r="I12" t="str">
             <v>(0.21)</v>
           </cell>
         </row>
-        <row r="654">
-          <cell r="A654" t="str">
+        <row r="18">
+          <cell r="A18" t="str">
             <v>R-sq</v>
           </cell>
-          <cell r="B654" t="str">
+          <cell r="B18" t="str">
             <v>0.012</v>
           </cell>
-          <cell r="C654" t="str">
+          <cell r="C18" t="str">
             <v>0.086</v>
           </cell>
-          <cell r="D654" t="str">
-            <v>0.010</v>
-          </cell>
-          <cell r="E654" t="str">
-            <v>0.035</v>
-          </cell>
-          <cell r="G654" t="str">
+          <cell r="D18" t="str">
+            <v>0.624</v>
+          </cell>
+          <cell r="E18" t="str">
+            <v>0.612</v>
+          </cell>
+          <cell r="G18" t="str">
             <v>0.078</v>
           </cell>
-          <cell r="I654" t="str">
+          <cell r="I18" t="str">
+            <v>0.606</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>DepVarMean</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>0.012</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>0.043</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>0.011</v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>0.036</v>
+          </cell>
+          <cell r="G19" t="str">
             <v>0.041</v>
           </cell>
-        </row>
-        <row r="655">
-          <cell r="A655" t="str">
-            <v>DepVarMean</v>
-          </cell>
-          <cell r="B655" t="str">
-            <v>0.012</v>
-          </cell>
-          <cell r="C655" t="str">
-            <v>0.043</v>
-          </cell>
-          <cell r="D655" t="str">
-            <v>0.012</v>
-          </cell>
-          <cell r="E655" t="str">
-            <v>0.043</v>
-          </cell>
-          <cell r="G655" t="str">
-            <v>0.041</v>
-          </cell>
-          <cell r="I655" t="str">
-            <v>0.041</v>
+          <cell r="I19" t="str">
+            <v>0.033</v>
           </cell>
         </row>
       </sheetData>
@@ -712,399 +703,388 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB048D4-D297-4E50-B32D-C65CD5E16CA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2817EF6B-0F34-4B17-9661-F96CD8A9247B}">
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G16"/>
+      <selection activeCell="G16" sqref="A2:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6"/>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="5" t="str">
         <f>[1]iv_reg_demand_pf!A2</f>
         <v/>
       </c>
-      <c r="B4" s="5" t="str">
+      <c r="B4" s="6" t="str">
         <f>[1]iv_reg_demand_pf!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C4" s="5" t="str">
+      <c r="C4" s="6" t="str">
         <f>[1]iv_reg_demand_pf!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="str">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="str">
         <f>[1]iv_reg_demand_pf!B5</f>
         <v>0.020</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="8" t="str">
         <f>[1]iv_reg_demand_pf!C5</f>
         <v/>
       </c>
-      <c r="D5" s="3" t="str">
+      <c r="D5" s="8" t="str">
         <f>[1]iv_reg_demand_pf!G5</f>
         <v/>
       </c>
-      <c r="E5" s="3" t="str">
+      <c r="E5" s="8" t="str">
         <f>[1]iv_reg_demand_pf!D5</f>
         <v>0.0100</v>
       </c>
-      <c r="F5" s="3" t="str">
+      <c r="F5" s="8" t="str">
         <f>[1]iv_reg_demand_pf!E5</f>
         <v/>
       </c>
-      <c r="G5" s="3" t="str">
+      <c r="G5" s="8" t="str">
         <f>[1]iv_reg_demand_pf!I5</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="str">
-        <f>[1]iv_reg_demand_pf!A6</f>
-        <v/>
-      </c>
-      <c r="B6" s="3" t="str">
+      <c r="B6" s="8" t="str">
         <f>[1]iv_reg_demand_pf!B6</f>
         <v>(0.00065)</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="8" t="str">
         <f>[1]iv_reg_demand_pf!C6</f>
         <v/>
       </c>
-      <c r="D6" s="3" t="str">
+      <c r="D6" s="8" t="str">
         <f>[1]iv_reg_demand_pf!G6</f>
         <v/>
       </c>
-      <c r="E6" s="3" t="str">
+      <c r="E6" s="8" t="str">
         <f>[1]iv_reg_demand_pf!D6</f>
         <v>(0.00084)</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="F6" s="8" t="str">
         <f>[1]iv_reg_demand_pf!E6</f>
         <v/>
       </c>
-      <c r="G6" s="3" t="str">
+      <c r="G6" s="8" t="str">
         <f>[1]iv_reg_demand_pf!I6</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!B644</f>
-        <v/>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!C644</f>
+        <v>4</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!B8</f>
+        <v/>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!C8</f>
         <v>0.49</v>
       </c>
-      <c r="D7" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!G644</f>
+      <c r="D7" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!G8</f>
         <v>0.42</v>
       </c>
-      <c r="E7" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!D644</f>
-        <v/>
-      </c>
-      <c r="F7" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!E644</f>
+      <c r="E7" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!D8</f>
+        <v/>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!E8</f>
         <v>0.30</v>
       </c>
-      <c r="G7" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!I644</f>
+      <c r="G7" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!I8</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="str">
-        <f>[1]iv_reg_demand_pf!A645</f>
-        <v/>
-      </c>
-      <c r="B8" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!B645</f>
-        <v/>
-      </c>
-      <c r="C8" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!C645</f>
+      <c r="B8" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!B9</f>
+        <v/>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!C9</f>
         <v>(0.071)</v>
       </c>
-      <c r="D8" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!G645</f>
+      <c r="D8" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!G9</f>
         <v>(0.076)</v>
       </c>
-      <c r="E8" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!D645</f>
-        <v/>
-      </c>
-      <c r="F8" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!E645</f>
+      <c r="E8" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!D9</f>
+        <v/>
+      </c>
+      <c r="F8" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!E9</f>
         <v>(0.18)</v>
       </c>
-      <c r="G8" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!I645</f>
+      <c r="G8" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!I9</f>
         <v>(0.21)</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!B647</f>
-        <v/>
-      </c>
-      <c r="C9" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!C647</f>
+        <v>5</v>
+      </c>
+      <c r="B9" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!B11</f>
+        <v/>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!C11</f>
         <v>-0.015</v>
       </c>
-      <c r="D9" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!G647</f>
+      <c r="D9" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!G11</f>
         <v>0.016</v>
       </c>
-      <c r="E9" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!D647</f>
-        <v/>
-      </c>
-      <c r="F9" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!E647</f>
+      <c r="E9" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!D11</f>
+        <v/>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!E11</f>
         <v>-0.51</v>
       </c>
-      <c r="G9" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!I647</f>
+      <c r="G9" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!I11</f>
         <v>-0.48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
-        <f>[1]iv_reg_demand_pf!A648</f>
-        <v/>
-      </c>
-      <c r="B10" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!B648</f>
-        <v/>
-      </c>
-      <c r="C10" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!C648</f>
+        <f>[1]iv_reg_demand_pf!A12</f>
+        <v/>
+      </c>
+      <c r="B10" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!B12</f>
+        <v/>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!C12</f>
         <v>(0.070)</v>
       </c>
-      <c r="D10" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!G648</f>
+      <c r="D10" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!G12</f>
         <v>(0.075)</v>
       </c>
-      <c r="E10" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!D648</f>
-        <v/>
-      </c>
-      <c r="F10" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!E648</f>
+      <c r="E10" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!D12</f>
+        <v/>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!E12</f>
         <v>(0.18)</v>
       </c>
-      <c r="G10" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!I648</f>
+      <c r="G10" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!I12</f>
         <v>(0.21)</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>18</v>
+      <c r="D11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0.7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
-        <f>[1]iv_reg_demand_pf!A654</f>
+        <f>[1]iv_reg_demand_pf!A18</f>
         <v>R-sq</v>
       </c>
-      <c r="B12" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!B654</f>
+      <c r="B12" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!B18</f>
         <v>0.012</v>
       </c>
-      <c r="C12" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!C654</f>
+      <c r="C12" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!C18</f>
         <v>0.086</v>
       </c>
-      <c r="D12" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!G654</f>
+      <c r="D12" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!G18</f>
         <v>0.078</v>
       </c>
-      <c r="E12" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!D654</f>
-        <v>0.010</v>
-      </c>
-      <c r="F12" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!E654</f>
-        <v>0.035</v>
-      </c>
-      <c r="G12" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!I654</f>
-        <v>0.041</v>
+      <c r="E12" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!D18</f>
+        <v>0.624</v>
+      </c>
+      <c r="F12" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!E18</f>
+        <v>0.612</v>
+      </c>
+      <c r="G12" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!I18</f>
+        <v>0.606</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
-        <f>[1]iv_reg_demand_pf!A655</f>
+        <f>[1]iv_reg_demand_pf!A19</f>
         <v>DepVarMean</v>
       </c>
-      <c r="B13" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!B655</f>
+      <c r="B13" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!B19</f>
         <v>0.012</v>
       </c>
-      <c r="C13" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!C655</f>
+      <c r="C13" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!C19</f>
         <v>0.043</v>
       </c>
-      <c r="D13" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!G655</f>
+      <c r="D13" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!G19</f>
         <v>0.041</v>
       </c>
-      <c r="E13" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!D655</f>
-        <v>0.012</v>
-      </c>
-      <c r="F13" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!E655</f>
-        <v>0.043</v>
-      </c>
-      <c r="G13" s="3" t="str">
-        <f>[1]iv_reg_demand_pf!I655</f>
-        <v>0.041</v>
+      <c r="E13" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!D19</f>
+        <v>0.011</v>
+      </c>
+      <c r="F13" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!E19</f>
+        <v>0.036</v>
+      </c>
+      <c r="G13" s="8" t="str">
+        <f>[1]iv_reg_demand_pf!I19</f>
+        <v>0.033</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
+      <c r="A14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>2</v>
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1113,7 +1093,6 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>